<commit_message>
added Geranium pusillum and Malva sylvestris to plant species
</commit_message>
<xml_diff>
--- a/butler_plants_risk.xlsx
+++ b/butler_plants_risk.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603A65BC-F84A-0E4A-A9E9-0447292B0994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38F2C20-5E89-2043-A7E2-BA60E3317D0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="1240" windowWidth="24440" windowHeight="12540" xr2:uid="{586401C8-9426-A049-BF32-66F51AAD1CB7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{586401C8-9426-A049-BF32-66F51AAD1CB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:B191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>